<commit_message>
trying to combine fetching format data with openpyxl and xlwings in object-oriented way not yet succeeded
</commit_message>
<xml_diff>
--- a/segments/format_test.xlsx
+++ b/segments/format_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nellie/Documenten/Python_programs/masterproef/openpyxl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nellie/Documenten/Python_programs/masterproef/segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE610DA-6F54-3A4F-9BBD-F29D5B170074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39AB7C8-2794-0B4A-80DE-D96641566E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14200" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
+    <workbookView xWindow="18800" yWindow="500" windowWidth="10000" windowHeight="16120" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>